<commit_message>
Sua loi chinh ta
</commit_message>
<xml_diff>
--- a/10_SRS/SRS_OpenLibrary.xlsx
+++ b/10_SRS/SRS_OpenLibrary.xlsx
@@ -18,11 +18,11 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="185">
   <si>
     <t>■Chi tiết</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■Mô tả</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -49,22 +49,22 @@
       </rPr>
       <t>ời dùng có thể tự tạo sách tiếng Nhật</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">Listup sách đã tạo </t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>(hoặc Hiển thị ban đầu)</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Trang chủ</t>
   </si>
   <si>
     <t>Trang chủ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -91,7 +91,7 @@
       </rPr>
       <t>ớng dẫn</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -118,28 +118,28 @@
       </rPr>
       <t xml:space="preserve"> viện tài liệu</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Bàn học</t>
   </si>
   <si>
     <t>Bàn học</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Giới thiệu</t>
   </si>
   <si>
     <t>Giới thiệu</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Liên hệ</t>
   </si>
   <si>
     <t>Liên hệ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -166,7 +166,7 @@
       </rPr>
       <t xml:space="preserve"> viện mở</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -193,11 +193,11 @@
       </rPr>
       <t>ớc khi sửa＞</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>＜Sau khi sửa＞</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Hướng dẫn</t>
@@ -223,27 +223,27 @@
   </si>
   <si>
     <t>Tên chức năng</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Mô tả giao diện</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Thêm 「Thư viện mở」 vào Menu bar (refer bên trái)</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">Khi nhấn vào link thì sẽ di chuyển đến màn hình </t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>chính của chức năng này.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>※Tham khảo [Listup sách đã tạo]</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -269,27 +269,27 @@
       </rPr>
       <t xml:space="preserve"> ← Click here</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tên sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Từ vựng</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Hành động</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>N4-5 vocabulary</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>No</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -316,35 +316,35 @@
       </rPr>
       <t>ợng thanh</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Kanji</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>N4_SakuraTT</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>N4_DongDu</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>No</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tên sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Hành động</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>※Chỉ người tạo + đối tượng được share mới thấy được</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -371,19 +371,19 @@
       </rPr>
       <t xml:space="preserve"> viện tài liêu」</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Sửa DB</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Nội dung xử lý</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Xử lý trên Webpage</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -410,7 +410,7 @@
       </rPr>
       <t>ợng share.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -437,7 +437,7 @@
       </rPr>
       <t>ời tạo sách.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -466,7 +466,7 @@
       </rPr>
       <t>ời tạo share cho.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -518,43 +518,43 @@
       </rPr>
       <t>ợng share mới thấy sách,</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Hiển thị ban đầu】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">   ・Hiển thị link 「Tạo sách mới」</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">   ・Hiển thị list các sách đã tạo, có phân loại.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【link 「Tạo sách mới」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">   ・Di chuyển sang màn hình tạo mới sách.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Sửa</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Xóa</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Chia xẻ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Hành động 「Sửa」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -581,39 +581,39 @@
       </rPr>
       <t>ng ứng.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Hành động 「Xóa」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">   ・Xóa sách trong Book TBL.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">   ・Reload lai màn hình hiện tại.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Danh sách các tài liệu bạn đã tạo</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tạo mới sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>1. Listup sách đã tạo.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>2. Tạo mới sách.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>3. Chỉnh sửa sách.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -640,11 +640,11 @@
       </rPr>
       <t xml:space="preserve"> viện mở」</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tạo link di chuyển Menu</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -671,7 +671,7 @@
       </rPr>
       <t xml:space="preserve"> viện mở」</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -698,7 +698,7 @@
       </rPr>
       <t xml:space="preserve"> viện mở].</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -725,7 +725,7 @@
       </rPr>
       <t xml:space="preserve"> viện mở」</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -752,126 +752,126 @@
       </rPr>
       <t xml:space="preserve"> viện mở].</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Hiển thị trên PC</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆jHiển thị trên SmartPhone</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Màn hình tạo sách mới</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Màn hình tạo nội dung cho sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Mô tả sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Cấp độ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Phân loại</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tag</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Phân loại(*)</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Cấp độ(*)</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tên sách(*)</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Từ vựng</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>N1</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t xml:space="preserve">Chỉ cần học kanji trong </t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>24h</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Nội dung</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Bài 1</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Chỉ cần học Kanji trong 24h</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Danh sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Ý nghĩa</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>うっかり</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>がっかり</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>24h_Word</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>{'level': 'N1', 'tag' : {'contains':',24h_Word,'}}</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Thất vọng, làm thất vọng</t>
   </si>
   <si>
     <t>Cách đọc:</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Ý nghĩa:</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Audio:</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Sample</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -898,11 +898,11 @@
       </rPr>
       <t>ng vẫn</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>がっかりしている。:</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>よく練習したのに、選手に選択されなかた為、</t>
@@ -915,7 +915,7 @@
     <rPh sb="12" eb="14">
       <t>センタク</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -942,39 +942,39 @@
       </rPr>
       <t>ợc chọn nên thất vọng.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Hiển thị ban đầu】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>All fields blank</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>[Tag] field sẽ tự động sinh ra, không cho phép input</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>24h_Word</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>{'level': 'N1', 'tag' : {'contains':',24h_Word,'}}</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【button 「Tiếp tục」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>mà sẽ di chuyển sang màn hình tạo nội dung cho sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【button 「Quay về」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1001,7 +1001,7 @@
       </rPr>
       <t xml:space="preserve"> viện mở)</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1025,7 +1025,7 @@
       </rPr>
       <t>※Tham khảo 「Tạo sách mới」</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1052,15 +1052,15 @@
       </rPr>
       <t>ớc</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・Vùng nội dung: All field blank</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【button 「Thêm」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1087,7 +1087,7 @@
       </rPr>
       <t>ớc đó.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1114,23 +1114,23 @@
       </rPr>
       <t>a đăng ký vao Book TBL ngay,</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Quay trở về màn hình listup sách đã tạo</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Link 「Tìm」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tìm kiếm audio từ DB hiện có.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Link 「Tạo」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1157,11 +1157,11 @@
       </rPr>
       <t>ời dùng tự</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>phát âm và record + upload.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1188,11 +1188,11 @@
       </rPr>
       <t>ời dùng Upload.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Link 「Lưu」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1219,7 +1219,7 @@
       </rPr>
       <t>u dữ liệu đã input tạm thời</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1246,23 +1246,23 @@
       </rPr>
       <t>u tạm thời</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Link 「Xóa」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Link 「Nhập lại」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Reset lại nội dung đã nhập</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【button 「Đăng ký」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1278,15 +1278,15 @@
       </rPr>
       <t>ưa nội dung Sách và Từ đã input lên cơ sở dữ liệu.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【button 「Hủy bỏ」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Cancel việc đăng ký, quay trở về màn hình chính</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1313,7 +1313,7 @@
       </rPr>
       <t xml:space="preserve"> viện mở.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1342,11 +1342,11 @@
       </rPr>
       <t xml:space="preserve">ng tự, chỉ </t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>khác nhau ở phần hiển thị input ở [Ý nghĩa]</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Chỉnh sửa sách.</t>
@@ -1373,11 +1373,11 @@
       </rPr>
       <t>※Tham khảo 「Chỉnh sửa sách」</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Màn hình chỉnh sửa sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1404,7 +1404,7 @@
       </rPr>
       <t>ợc hiển thị</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1431,39 +1431,39 @@
       </rPr>
       <t>u thay đổi không/cancel)</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Di chuyển sang màn hình chỉnh sửa nội dung sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>◆Màn hình chỉnh sửa nội dung cho sách</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Cho phép nhập từ ở dòng mới.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・Vùng nội dung: Hiển thị thông tin từ DB</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【button 「Sửa」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Enable sửa ở line đang có focus.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【button 「Sửa DB」】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Đăng ký lại Sách và Từ đã input lên cơ sở dữ liệu.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1482,43 +1482,43 @@
       </rPr>
       <t>24h_Word</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Nino49a</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Tugigroup</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>YYY</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Nino49a</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Thanhnv</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>XXX</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>TuyenTuyen</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>All account</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Share account</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1545,11 +1545,11 @@
       </rPr>
       <t>ợc sách.</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・Tên sách hiển thị</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1576,23 +1576,23 @@
       </rPr>
       <t>ời dùng hiển thị</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・Share account: Blank</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>【Thao tác】</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>All account: Chọn Account muốn share &amp; click [&gt;&gt;]</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Share Account: Chọn Account muốn cắt share &amp; click [&lt;&lt;]</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1618,7 +1618,7 @@
       </rPr>
       <t>」】</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1645,11 +1645,11 @@
       </rPr>
       <t>ợc đăng ký vào 「PublicTo」</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>trong Book TBL.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1665,11 +1665,11 @@
       </rPr>
       <t>」】</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Hủy bỏ share book và quay về màn hình chính.</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1698,7 +1698,7 @@
       </rPr>
       <t>ợc share cho</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -1714,7 +1714,7 @@
       </rPr>
       <t>c account có sẵn đó</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>&amp; Chia sẻ với các người dùng khác.</t>
@@ -1739,13 +1739,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2145,7 +2152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -2178,25 +2185,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
@@ -2208,10 +2215,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1">
@@ -2223,34 +2230,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2262,7 +2269,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1">
@@ -2313,13 +2320,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
@@ -2337,7 +2344,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1">
@@ -2349,67 +2356,70 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2420,9 +2430,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2940,7 +2947,7 @@
             <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
-              <a:t>Chia xẻ với bạn bè </a:t>
+              <a:t>Chia sẻ với bạn bè </a:t>
             </a:r>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
           </a:p>
@@ -14405,7 +14412,7 @@
       <c r="X189" s="4"/>
       <c r="Y189" s="4"/>
       <c r="Z189" s="5"/>
-      <c r="AA189" s="90" t="s">
+      <c r="AA189" s="87" t="s">
         <v>178</v>
       </c>
       <c r="AB189" s="4"/>
@@ -14659,7 +14666,7 @@
       <c r="X195" s="4"/>
       <c r="Y195" s="4"/>
       <c r="Z195" s="5"/>
-      <c r="AA195" s="90" t="s">
+      <c r="AA195" s="87" t="s">
         <v>172</v>
       </c>
       <c r="AB195" s="4"/>
@@ -14829,7 +14836,7 @@
       <c r="X199" s="4"/>
       <c r="Y199" s="4"/>
       <c r="Z199" s="5"/>
-      <c r="AA199" s="90" t="s">
+      <c r="AA199" s="87" t="s">
         <v>175</v>
       </c>
       <c r="AB199" s="4"/>
@@ -15218,7 +15225,7 @@
       <c r="AN208" s="18"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <hyperlinks>
     <hyperlink ref="AA36:AH36" location="SRS!A34" display="※Tham khảo [Listup sách đã tạo]"/>
     <hyperlink ref="AA75:AG75" location="SRS!B89" display="   ※Tham khảo 「Tạo sách mới」"/>
@@ -15593,7 +15600,7 @@
       </c>
       <c r="AC25" s="3"/>
       <c r="AD25" s="4"/>
-      <c r="AE25" s="87" t="s">
+      <c r="AE25" s="88" t="s">
         <v>77</v>
       </c>
       <c r="AF25" s="34" t="s">
@@ -15609,7 +15616,7 @@
       </c>
       <c r="BK25" s="3"/>
       <c r="BL25" s="4"/>
-      <c r="BM25" s="87" t="s">
+      <c r="BM25" s="88" t="s">
         <v>77</v>
       </c>
       <c r="BN25" s="34" t="s">
@@ -15627,7 +15634,7 @@
       </c>
       <c r="AC26" s="36"/>
       <c r="AD26" s="4"/>
-      <c r="AE26" s="88"/>
+      <c r="AE26" s="89"/>
       <c r="AF26" s="35" t="s">
         <v>87</v>
       </c>
@@ -15641,7 +15648,7 @@
       </c>
       <c r="BK26" s="36"/>
       <c r="BL26" s="4"/>
-      <c r="BM26" s="88"/>
+      <c r="BM26" s="89"/>
       <c r="BN26" s="35" t="s">
         <v>87</v>
       </c>
@@ -15657,7 +15664,7 @@
       </c>
       <c r="AC27" s="36"/>
       <c r="AD27" s="4"/>
-      <c r="AE27" s="88"/>
+      <c r="AE27" s="89"/>
       <c r="AF27" s="35"/>
       <c r="AG27" s="5"/>
       <c r="BH27" s="6"/>
@@ -15669,7 +15676,7 @@
       </c>
       <c r="BK27" s="36"/>
       <c r="BL27" s="4"/>
-      <c r="BM27" s="88"/>
+      <c r="BM27" s="89"/>
       <c r="BN27" s="35"/>
       <c r="BO27" s="5"/>
     </row>
@@ -15683,7 +15690,7 @@
       </c>
       <c r="AC28" s="38"/>
       <c r="AD28" s="4"/>
-      <c r="AE28" s="89"/>
+      <c r="AE28" s="90"/>
       <c r="AF28" s="36"/>
       <c r="AG28" s="5"/>
       <c r="BH28" s="53"/>
@@ -15695,7 +15702,7 @@
       </c>
       <c r="BK28" s="38"/>
       <c r="BL28" s="4"/>
-      <c r="BM28" s="89"/>
+      <c r="BM28" s="90"/>
       <c r="BN28" s="36"/>
       <c r="BO28" s="53"/>
     </row>
@@ -15872,7 +15879,7 @@
       <c r="AT35" s="41"/>
       <c r="AU35" s="38"/>
       <c r="AV35" s="4"/>
-      <c r="AW35" s="87" t="s">
+      <c r="AW35" s="88" t="s">
         <v>77</v>
       </c>
       <c r="AX35" s="43" t="s">
@@ -15903,7 +15910,7 @@
       <c r="CB35" s="41"/>
       <c r="CC35" s="38"/>
       <c r="CD35" s="4"/>
-      <c r="CE35" s="87" t="s">
+      <c r="CE35" s="88" t="s">
         <v>77</v>
       </c>
       <c r="CF35" s="43" t="s">
@@ -15936,7 +15943,7 @@
       <c r="AT36" s="41"/>
       <c r="AU36" s="38"/>
       <c r="AV36" s="4"/>
-      <c r="AW36" s="88"/>
+      <c r="AW36" s="89"/>
       <c r="AX36" s="46"/>
       <c r="AY36" s="47"/>
       <c r="AZ36" s="47"/>
@@ -15963,7 +15970,7 @@
       <c r="CB36" s="41"/>
       <c r="CC36" s="38"/>
       <c r="CD36" s="4"/>
-      <c r="CE36" s="88"/>
+      <c r="CE36" s="89"/>
       <c r="CF36" s="46"/>
       <c r="CG36" s="47"/>
       <c r="CH36" s="47"/>
@@ -15992,7 +15999,7 @@
       <c r="AT37" s="41"/>
       <c r="AU37" s="38"/>
       <c r="AV37" s="4"/>
-      <c r="AW37" s="88"/>
+      <c r="AW37" s="89"/>
       <c r="AX37" s="46"/>
       <c r="AY37" s="47"/>
       <c r="AZ37" s="47"/>
@@ -16019,7 +16026,7 @@
       <c r="CB37" s="41"/>
       <c r="CC37" s="38"/>
       <c r="CD37" s="4"/>
-      <c r="CE37" s="88"/>
+      <c r="CE37" s="89"/>
       <c r="CF37" s="46"/>
       <c r="CG37" s="47"/>
       <c r="CH37" s="47"/>
@@ -16048,7 +16055,7 @@
       <c r="AT38" s="41"/>
       <c r="AU38" s="38"/>
       <c r="AV38" s="4"/>
-      <c r="AW38" s="89"/>
+      <c r="AW38" s="90"/>
       <c r="AX38" s="48"/>
       <c r="AY38" s="49"/>
       <c r="AZ38" s="49"/>
@@ -16075,7 +16082,7 @@
       <c r="CB38" s="41"/>
       <c r="CC38" s="38"/>
       <c r="CD38" s="4"/>
-      <c r="CE38" s="89"/>
+      <c r="CE38" s="90"/>
       <c r="CF38" s="48"/>
       <c r="CG38" s="49"/>
       <c r="CH38" s="49"/>
@@ -17422,7 +17429,7 @@
     <mergeCell ref="BM25:BM28"/>
     <mergeCell ref="CE35:CE38"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <hyperlinks>
     <hyperlink ref="DB62" r:id="rId1" display="Nino49a@gmail.com"/>
     <hyperlink ref="DB63" r:id="rId2" display="Tugigroup@gmail.com"/>

</xml_diff>